<commit_message>
Latest financials from £JOUL, add news events
</commit_message>
<xml_diff>
--- a/£JOUL.xlsx
+++ b/£JOUL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20391"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Stocks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{459D64B4-8BF9-4C9F-8002-39976AA6C5CA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD721FF3-2080-954D-AA4F-7CD2A4878504}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28215" windowHeight="10275" activeTab="1" xr2:uid="{C3D898C5-A016-4C72-B082-1E1424AE10EB}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18900" activeTab="1" xr2:uid="{C3D898C5-A016-4C72-B082-1E1424AE10EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -21,12 +21,22 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="91">
   <si>
     <t>£JOUL</t>
   </si>
@@ -274,16 +284,41 @@
     <t>Book Value per Share</t>
   </si>
   <si>
-    <t>Invento</t>
+    <t>Inventory Y/Y</t>
+  </si>
+  <si>
+    <t>Inventory H/H</t>
+  </si>
+  <si>
+    <t>Share Price</t>
+  </si>
+  <si>
+    <t>P/B</t>
+  </si>
+  <si>
+    <t>P/S</t>
+  </si>
+  <si>
+    <t>EV/S</t>
+  </si>
+  <si>
+    <t>P/E</t>
+  </si>
+  <si>
+    <t>EV/E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Joule's open new £20m headquarters in Market Harborough </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
-    <numFmt numFmtId="171" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="168" formatCode="0.0\x"/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
@@ -491,19 +526,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -531,30 +557,10 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="15" fontId="4" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -566,12 +572,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -596,12 +596,64 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="171" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="171" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="2" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -698,8 +750,8 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -714,8 +766,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7086600" y="9525"/>
-          <a:ext cx="0" cy="8153400"/>
+          <a:off x="9039225" y="9525"/>
+          <a:ext cx="0" cy="14481175"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -748,8 +800,8 @@
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -764,8 +816,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11963400" y="0"/>
-          <a:ext cx="0" cy="8153400"/>
+          <a:off x="14627225" y="0"/>
+          <a:ext cx="0" cy="14592300"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1091,682 +1143,714 @@
   <dimension ref="A2:S37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="C26" sqref="C26:D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:19" ht="15" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="23"/>
-    </row>
-    <row r="3" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="E2" s="18"/>
+    </row>
+    <row r="3" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B5" s="3" t="s">
+    <row r="5" spans="2:19" x14ac:dyDescent="0.15">
+      <c r="B5" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="5"/>
-      <c r="G5" s="3" t="s">
+      <c r="C5" s="48"/>
+      <c r="D5" s="49"/>
+      <c r="G5" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
-      <c r="P5" s="4"/>
-      <c r="Q5" s="4"/>
-      <c r="R5" s="4"/>
-      <c r="S5" s="5"/>
-    </row>
-    <row r="6" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B6" s="6" t="s">
+      <c r="H5" s="48"/>
+      <c r="I5" s="48"/>
+      <c r="J5" s="48"/>
+      <c r="K5" s="48"/>
+      <c r="L5" s="48"/>
+      <c r="M5" s="48"/>
+      <c r="N5" s="48"/>
+      <c r="O5" s="48"/>
+      <c r="P5" s="48"/>
+      <c r="Q5" s="48"/>
+      <c r="R5" s="48"/>
+      <c r="S5" s="49"/>
+    </row>
+    <row r="6" spans="2:19" x14ac:dyDescent="0.15">
+      <c r="B6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="4">
         <v>9.2200000000000004E-2</v>
       </c>
-      <c r="D6" s="9"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="14"/>
-      <c r="M6" s="14"/>
-      <c r="N6" s="14"/>
-      <c r="O6" s="14"/>
-      <c r="P6" s="14"/>
-      <c r="Q6" s="14"/>
-      <c r="R6" s="14"/>
-      <c r="S6" s="15"/>
-    </row>
-    <row r="7" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B7" s="6" t="s">
+      <c r="D6" s="6"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="11"/>
+      <c r="P6" s="11"/>
+      <c r="Q6" s="11"/>
+      <c r="R6" s="11"/>
+      <c r="S6" s="12"/>
+    </row>
+    <row r="7" spans="2:19" x14ac:dyDescent="0.15">
+      <c r="B7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="11">
-        <v>112.09</v>
-      </c>
-      <c r="D7" s="9"/>
-      <c r="G7" s="24">
+      <c r="C7" s="8">
+        <f>'Financial Model'!K16</f>
+        <v>110.3</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" s="19">
         <v>44879</v>
       </c>
-      <c r="H7" s="14" t="s">
+      <c r="H7" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="14"/>
-      <c r="M7" s="14"/>
-      <c r="N7" s="14"/>
-      <c r="O7" s="14"/>
-      <c r="P7" s="14"/>
-      <c r="Q7" s="14"/>
-      <c r="R7" s="14"/>
-      <c r="S7" s="15"/>
-    </row>
-    <row r="8" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B8" s="6" t="s">
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="11"/>
+      <c r="O7" s="11"/>
+      <c r="P7" s="11"/>
+      <c r="Q7" s="11"/>
+      <c r="R7" s="11"/>
+      <c r="S7" s="12"/>
+    </row>
+    <row r="8" spans="2:19" x14ac:dyDescent="0.15">
+      <c r="B8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="11">
+      <c r="C8" s="8">
         <f>C6*C7</f>
-        <v>10.334698000000001</v>
-      </c>
-      <c r="D8" s="9"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="14"/>
-      <c r="M8" s="14"/>
-      <c r="N8" s="14"/>
-      <c r="O8" s="14"/>
-      <c r="P8" s="14"/>
-      <c r="Q8" s="14"/>
-      <c r="R8" s="14"/>
-      <c r="S8" s="15"/>
-    </row>
-    <row r="9" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B9" s="6" t="s">
+        <v>10.16966</v>
+      </c>
+      <c r="D8" s="6"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="11"/>
+      <c r="O8" s="11"/>
+      <c r="P8" s="11"/>
+      <c r="Q8" s="11"/>
+      <c r="R8" s="11"/>
+      <c r="S8" s="12"/>
+    </row>
+    <row r="9" spans="2:19" x14ac:dyDescent="0.15">
+      <c r="B9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="11"/>
-      <c r="D9" s="9"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="14"/>
-      <c r="M9" s="14"/>
-      <c r="N9" s="14"/>
-      <c r="O9" s="14"/>
-      <c r="P9" s="14"/>
-      <c r="Q9" s="14"/>
-      <c r="R9" s="14"/>
-      <c r="S9" s="15"/>
-    </row>
-    <row r="10" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B10" s="6" t="s">
+      <c r="C9" s="8">
+        <f>'Financial Model'!K68</f>
+        <v>19.350999999999999</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G9" s="16"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="11"/>
+      <c r="O9" s="11"/>
+      <c r="P9" s="11"/>
+      <c r="Q9" s="11"/>
+      <c r="R9" s="11"/>
+      <c r="S9" s="12"/>
+    </row>
+    <row r="10" spans="2:19" x14ac:dyDescent="0.15">
+      <c r="B10" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="11"/>
-      <c r="D10" s="9"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="14"/>
-      <c r="M10" s="14"/>
-      <c r="N10" s="14"/>
-      <c r="O10" s="14"/>
-      <c r="P10" s="14"/>
-      <c r="Q10" s="14"/>
-      <c r="R10" s="14"/>
-      <c r="S10" s="15"/>
-    </row>
-    <row r="11" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B11" s="6" t="s">
+      <c r="C10" s="8">
+        <f>'Financial Model'!K69</f>
+        <v>25.856000000000002</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G10" s="16"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="11"/>
+      <c r="N10" s="11"/>
+      <c r="O10" s="11"/>
+      <c r="P10" s="11"/>
+      <c r="Q10" s="11"/>
+      <c r="R10" s="11"/>
+      <c r="S10" s="12"/>
+    </row>
+    <row r="11" spans="2:19" x14ac:dyDescent="0.15">
+      <c r="B11" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="11">
+      <c r="C11" s="8">
         <f>C9-C10</f>
-        <v>0</v>
-      </c>
-      <c r="D11" s="9"/>
-      <c r="G11" s="19"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="14"/>
-      <c r="L11" s="14"/>
-      <c r="M11" s="14"/>
-      <c r="N11" s="14"/>
-      <c r="O11" s="14"/>
-      <c r="P11" s="14"/>
-      <c r="Q11" s="14"/>
-      <c r="R11" s="14"/>
-      <c r="S11" s="15"/>
-    </row>
-    <row r="12" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B12" s="8" t="s">
+        <v>-6.5050000000000026</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G11" s="16"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="11"/>
+      <c r="O11" s="11"/>
+      <c r="P11" s="11"/>
+      <c r="Q11" s="11"/>
+      <c r="R11" s="11"/>
+      <c r="S11" s="12"/>
+    </row>
+    <row r="12" spans="2:19" x14ac:dyDescent="0.15">
+      <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="12">
+      <c r="C12" s="9">
         <f>C8-C11</f>
-        <v>10.334698000000001</v>
-      </c>
-      <c r="D12" s="10"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="14"/>
-      <c r="L12" s="14"/>
-      <c r="M12" s="14"/>
-      <c r="N12" s="14"/>
-      <c r="O12" s="14"/>
-      <c r="P12" s="14"/>
-      <c r="Q12" s="14"/>
-      <c r="R12" s="14"/>
-      <c r="S12" s="15"/>
-    </row>
-    <row r="13" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="G13" s="19"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="14"/>
-      <c r="M13" s="14"/>
-      <c r="N13" s="14"/>
-      <c r="O13" s="14"/>
-      <c r="P13" s="14"/>
-      <c r="Q13" s="14"/>
-      <c r="R13" s="14"/>
-      <c r="S13" s="15"/>
-    </row>
-    <row r="14" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="G14" s="19"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="14"/>
-      <c r="L14" s="14"/>
-      <c r="M14" s="14"/>
-      <c r="N14" s="14"/>
-      <c r="O14" s="14"/>
-      <c r="P14" s="14"/>
-      <c r="Q14" s="14"/>
-      <c r="R14" s="14"/>
-      <c r="S14" s="15"/>
-    </row>
-    <row r="15" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B15" s="3" t="s">
+        <v>16.674660000000003</v>
+      </c>
+      <c r="D12" s="7"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="11"/>
+      <c r="N12" s="11"/>
+      <c r="O12" s="11"/>
+      <c r="P12" s="11"/>
+      <c r="Q12" s="11"/>
+      <c r="R12" s="11"/>
+      <c r="S12" s="12"/>
+    </row>
+    <row r="13" spans="2:19" x14ac:dyDescent="0.15">
+      <c r="G13" s="16"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
+      <c r="M13" s="11"/>
+      <c r="N13" s="11"/>
+      <c r="O13" s="11"/>
+      <c r="P13" s="11"/>
+      <c r="Q13" s="11"/>
+      <c r="R13" s="11"/>
+      <c r="S13" s="12"/>
+    </row>
+    <row r="14" spans="2:19" x14ac:dyDescent="0.15">
+      <c r="G14" s="16"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="11"/>
+      <c r="M14" s="11"/>
+      <c r="N14" s="11"/>
+      <c r="O14" s="11"/>
+      <c r="P14" s="11"/>
+      <c r="Q14" s="11"/>
+      <c r="R14" s="11"/>
+      <c r="S14" s="12"/>
+    </row>
+    <row r="15" spans="2:19" x14ac:dyDescent="0.15">
+      <c r="B15" s="47" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="5"/>
-      <c r="G15" s="19"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="14"/>
-      <c r="M15" s="14"/>
-      <c r="N15" s="14"/>
-      <c r="O15" s="14"/>
-      <c r="P15" s="14"/>
-      <c r="Q15" s="14"/>
-      <c r="R15" s="14"/>
-      <c r="S15" s="15"/>
-    </row>
-    <row r="16" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B16" s="13" t="s">
+      <c r="C15" s="48"/>
+      <c r="D15" s="49"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="11"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="11"/>
+      <c r="L15" s="11"/>
+      <c r="M15" s="11"/>
+      <c r="N15" s="11"/>
+      <c r="O15" s="11"/>
+      <c r="P15" s="11"/>
+      <c r="Q15" s="11"/>
+      <c r="R15" s="11"/>
+      <c r="S15" s="12"/>
+    </row>
+    <row r="16" spans="2:19" x14ac:dyDescent="0.15">
+      <c r="B16" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="25" t="s">
+      <c r="C16" s="41" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="26"/>
-      <c r="G16" s="19"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="14"/>
-      <c r="L16" s="14"/>
-      <c r="M16" s="14"/>
-      <c r="N16" s="14"/>
-      <c r="O16" s="14"/>
-      <c r="P16" s="14"/>
-      <c r="Q16" s="14"/>
-      <c r="R16" s="14"/>
-      <c r="S16" s="15"/>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="B17" s="13" t="s">
+      <c r="D16" s="42"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="11"/>
+      <c r="M16" s="11"/>
+      <c r="N16" s="11"/>
+      <c r="O16" s="11"/>
+      <c r="P16" s="11"/>
+      <c r="Q16" s="11"/>
+      <c r="R16" s="11"/>
+      <c r="S16" s="12"/>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="B17" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="25" t="s">
+      <c r="C17" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="D17" s="26"/>
-      <c r="G17" s="19"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="14"/>
-      <c r="L17" s="14"/>
-      <c r="M17" s="14"/>
-      <c r="N17" s="14"/>
-      <c r="O17" s="14"/>
-      <c r="P17" s="14"/>
-      <c r="Q17" s="14"/>
-      <c r="R17" s="14"/>
-      <c r="S17" s="15"/>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="B18" s="13" t="s">
+      <c r="D17" s="42"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="11"/>
+      <c r="L17" s="11"/>
+      <c r="M17" s="11"/>
+      <c r="N17" s="11"/>
+      <c r="O17" s="11"/>
+      <c r="P17" s="11"/>
+      <c r="Q17" s="11"/>
+      <c r="R17" s="11"/>
+      <c r="S17" s="12"/>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="B18" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="25"/>
-      <c r="D18" s="26"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="14"/>
-      <c r="K18" s="14"/>
-      <c r="L18" s="14"/>
-      <c r="M18" s="14"/>
-      <c r="N18" s="14"/>
-      <c r="O18" s="14"/>
-      <c r="P18" s="14"/>
-      <c r="Q18" s="14"/>
-      <c r="R18" s="14"/>
-      <c r="S18" s="15"/>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A19" s="31" t="s">
+      <c r="C18" s="41"/>
+      <c r="D18" s="42"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="11"/>
+      <c r="M18" s="11"/>
+      <c r="N18" s="11"/>
+      <c r="O18" s="11"/>
+      <c r="P18" s="11"/>
+      <c r="Q18" s="11"/>
+      <c r="R18" s="11"/>
+      <c r="S18" s="12"/>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A19" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="B19" s="16" t="s">
+      <c r="B19" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="27" t="s">
+      <c r="C19" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="D19" s="28"/>
-      <c r="G19" s="19"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="14"/>
-      <c r="K19" s="14"/>
-      <c r="L19" s="14"/>
-      <c r="M19" s="14"/>
-      <c r="N19" s="14"/>
-      <c r="O19" s="14"/>
-      <c r="P19" s="14"/>
-      <c r="Q19" s="14"/>
-      <c r="R19" s="14"/>
-      <c r="S19" s="15"/>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="G20" s="19"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="14"/>
-      <c r="K20" s="14"/>
-      <c r="L20" s="14"/>
-      <c r="M20" s="14"/>
-      <c r="N20" s="14"/>
-      <c r="O20" s="14"/>
-      <c r="P20" s="14"/>
-      <c r="Q20" s="14"/>
-      <c r="R20" s="14"/>
-      <c r="S20" s="15"/>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="G21" s="19"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="14"/>
-      <c r="K21" s="14"/>
-      <c r="L21" s="14"/>
-      <c r="M21" s="14"/>
-      <c r="N21" s="14"/>
-      <c r="O21" s="14"/>
-      <c r="P21" s="14"/>
-      <c r="Q21" s="14"/>
-      <c r="R21" s="14"/>
-      <c r="S21" s="15"/>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="B22" s="3" t="s">
+      <c r="D19" s="44"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="11"/>
+      <c r="L19" s="11"/>
+      <c r="M19" s="11"/>
+      <c r="N19" s="11"/>
+      <c r="O19" s="11"/>
+      <c r="P19" s="11"/>
+      <c r="Q19" s="11"/>
+      <c r="R19" s="11"/>
+      <c r="S19" s="12"/>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="G20" s="16"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="11"/>
+      <c r="L20" s="11"/>
+      <c r="M20" s="11"/>
+      <c r="N20" s="11"/>
+      <c r="O20" s="11"/>
+      <c r="P20" s="11"/>
+      <c r="Q20" s="11"/>
+      <c r="R20" s="11"/>
+      <c r="S20" s="12"/>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="G21" s="16"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="11"/>
+      <c r="K21" s="11"/>
+      <c r="L21" s="11"/>
+      <c r="M21" s="11"/>
+      <c r="N21" s="11"/>
+      <c r="O21" s="11"/>
+      <c r="P21" s="11"/>
+      <c r="Q21" s="11"/>
+      <c r="R21" s="11"/>
+      <c r="S21" s="12"/>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="B22" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="C22" s="4"/>
-      <c r="D22" s="5"/>
-      <c r="G22" s="19"/>
-      <c r="H22" s="14"/>
-      <c r="I22" s="14"/>
-      <c r="J22" s="14"/>
-      <c r="K22" s="14"/>
-      <c r="L22" s="14"/>
-      <c r="M22" s="14"/>
-      <c r="N22" s="14"/>
-      <c r="O22" s="14"/>
-      <c r="P22" s="14"/>
-      <c r="Q22" s="14"/>
-      <c r="R22" s="14"/>
-      <c r="S22" s="15"/>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="B23" s="19" t="s">
+      <c r="C22" s="48"/>
+      <c r="D22" s="49"/>
+      <c r="G22" s="57">
+        <v>44508</v>
+      </c>
+      <c r="H22" s="58" t="s">
+        <v>90</v>
+      </c>
+      <c r="I22" s="11"/>
+      <c r="J22" s="11"/>
+      <c r="K22" s="11"/>
+      <c r="L22" s="11"/>
+      <c r="M22" s="11"/>
+      <c r="N22" s="11"/>
+      <c r="O22" s="11"/>
+      <c r="P22" s="11"/>
+      <c r="Q22" s="11"/>
+      <c r="R22" s="11"/>
+      <c r="S22" s="12"/>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="B23" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="C23" s="25" t="s">
+      <c r="C23" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="D23" s="26"/>
-      <c r="G23" s="19"/>
-      <c r="H23" s="14"/>
-      <c r="I23" s="14"/>
-      <c r="J23" s="14"/>
-      <c r="K23" s="14"/>
-      <c r="L23" s="14"/>
-      <c r="M23" s="14"/>
-      <c r="N23" s="14"/>
-      <c r="O23" s="14"/>
-      <c r="P23" s="14"/>
-      <c r="Q23" s="14"/>
-      <c r="R23" s="14"/>
-      <c r="S23" s="15"/>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="B24" s="19" t="s">
+      <c r="D23" s="42"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="11"/>
+      <c r="J23" s="11"/>
+      <c r="K23" s="11"/>
+      <c r="L23" s="11"/>
+      <c r="M23" s="11"/>
+      <c r="N23" s="11"/>
+      <c r="O23" s="11"/>
+      <c r="P23" s="11"/>
+      <c r="Q23" s="11"/>
+      <c r="R23" s="11"/>
+      <c r="S23" s="12"/>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="B24" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C24" s="25">
+      <c r="C24" s="41">
         <v>1989</v>
       </c>
-      <c r="D24" s="26"/>
-      <c r="G24" s="19"/>
-      <c r="H24" s="14"/>
-      <c r="I24" s="14"/>
-      <c r="J24" s="14"/>
-      <c r="K24" s="14"/>
-      <c r="L24" s="14"/>
-      <c r="M24" s="14"/>
-      <c r="N24" s="14"/>
-      <c r="O24" s="14"/>
-      <c r="P24" s="14"/>
-      <c r="Q24" s="14"/>
-      <c r="R24" s="14"/>
-      <c r="S24" s="15"/>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="B25" s="19"/>
-      <c r="C25" s="25"/>
-      <c r="D25" s="26"/>
-      <c r="G25" s="19"/>
-      <c r="H25" s="14"/>
-      <c r="I25" s="14"/>
-      <c r="J25" s="14"/>
-      <c r="K25" s="14"/>
-      <c r="L25" s="14"/>
-      <c r="M25" s="14"/>
-      <c r="N25" s="14"/>
-      <c r="O25" s="14"/>
-      <c r="P25" s="14"/>
-      <c r="Q25" s="14"/>
-      <c r="R25" s="14"/>
-      <c r="S25" s="15"/>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="B26" s="19" t="s">
+      <c r="D24" s="42"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="11"/>
+      <c r="K24" s="11"/>
+      <c r="L24" s="11"/>
+      <c r="M24" s="11"/>
+      <c r="N24" s="11"/>
+      <c r="O24" s="11"/>
+      <c r="P24" s="11"/>
+      <c r="Q24" s="11"/>
+      <c r="R24" s="11"/>
+      <c r="S24" s="12"/>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="B25" s="16"/>
+      <c r="C25" s="41"/>
+      <c r="D25" s="42"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="11"/>
+      <c r="K25" s="11"/>
+      <c r="L25" s="11"/>
+      <c r="M25" s="11"/>
+      <c r="N25" s="11"/>
+      <c r="O25" s="11"/>
+      <c r="P25" s="11"/>
+      <c r="Q25" s="11"/>
+      <c r="R25" s="11"/>
+      <c r="S25" s="12"/>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="B26" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C26" s="25"/>
-      <c r="D26" s="26"/>
-      <c r="G26" s="19"/>
-      <c r="H26" s="14"/>
-      <c r="I26" s="14"/>
-      <c r="J26" s="14"/>
-      <c r="K26" s="14"/>
-      <c r="L26" s="14"/>
-      <c r="M26" s="14"/>
-      <c r="N26" s="14"/>
-      <c r="O26" s="14"/>
-      <c r="P26" s="14"/>
-      <c r="Q26" s="14"/>
-      <c r="R26" s="14"/>
-      <c r="S26" s="15"/>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="B27" s="19"/>
-      <c r="C27" s="25"/>
-      <c r="D27" s="26"/>
-      <c r="G27" s="19"/>
-      <c r="H27" s="14"/>
-      <c r="I27" s="14"/>
-      <c r="J27" s="14"/>
-      <c r="K27" s="14"/>
-      <c r="L27" s="14"/>
-      <c r="M27" s="14"/>
-      <c r="N27" s="14"/>
-      <c r="O27" s="14"/>
-      <c r="P27" s="14"/>
-      <c r="Q27" s="14"/>
-      <c r="R27" s="14"/>
-      <c r="S27" s="15"/>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="B28" s="19" t="s">
+      <c r="C26" s="59">
+        <f>'Financial Model'!K35</f>
+        <v>61.878</v>
+      </c>
+      <c r="D26" s="60"/>
+      <c r="G26" s="16"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="11"/>
+      <c r="J26" s="11"/>
+      <c r="K26" s="11"/>
+      <c r="L26" s="11"/>
+      <c r="M26" s="11"/>
+      <c r="N26" s="11"/>
+      <c r="O26" s="11"/>
+      <c r="P26" s="11"/>
+      <c r="Q26" s="11"/>
+      <c r="R26" s="11"/>
+      <c r="S26" s="12"/>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="B27" s="16"/>
+      <c r="C27" s="41"/>
+      <c r="D27" s="42"/>
+      <c r="G27" s="16"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="11"/>
+      <c r="J27" s="11"/>
+      <c r="K27" s="11"/>
+      <c r="L27" s="11"/>
+      <c r="M27" s="11"/>
+      <c r="N27" s="11"/>
+      <c r="O27" s="11"/>
+      <c r="P27" s="11"/>
+      <c r="Q27" s="11"/>
+      <c r="R27" s="11"/>
+      <c r="S27" s="12"/>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="B28" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="C28" s="29"/>
-      <c r="D28" s="30"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="14"/>
-      <c r="I28" s="14"/>
-      <c r="J28" s="14"/>
-      <c r="K28" s="14"/>
-      <c r="L28" s="14"/>
-      <c r="M28" s="14"/>
-      <c r="N28" s="14"/>
-      <c r="O28" s="14"/>
-      <c r="P28" s="14"/>
-      <c r="Q28" s="14"/>
-      <c r="R28" s="14"/>
-      <c r="S28" s="15"/>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="B29" s="20" t="s">
+      <c r="C28" s="55" t="s">
+        <v>30</v>
+      </c>
+      <c r="D28" s="56">
+        <v>44600</v>
+      </c>
+      <c r="G28" s="16"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="11"/>
+      <c r="J28" s="11"/>
+      <c r="K28" s="11"/>
+      <c r="L28" s="11"/>
+      <c r="M28" s="11"/>
+      <c r="N28" s="11"/>
+      <c r="O28" s="11"/>
+      <c r="P28" s="11"/>
+      <c r="Q28" s="11"/>
+      <c r="R28" s="11"/>
+      <c r="S28" s="12"/>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="B29" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C29" s="35" t="s">
+      <c r="C29" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="D29" s="36"/>
-      <c r="G29" s="19"/>
-      <c r="H29" s="14"/>
-      <c r="I29" s="14"/>
-      <c r="J29" s="14"/>
-      <c r="K29" s="14"/>
-      <c r="L29" s="14"/>
-      <c r="M29" s="14"/>
-      <c r="N29" s="14"/>
-      <c r="O29" s="14"/>
-      <c r="P29" s="14"/>
-      <c r="Q29" s="14"/>
-      <c r="R29" s="14"/>
-      <c r="S29" s="15"/>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="G30" s="19"/>
-      <c r="H30" s="14"/>
-      <c r="I30" s="14"/>
-      <c r="J30" s="14"/>
-      <c r="K30" s="14"/>
-      <c r="L30" s="14"/>
-      <c r="M30" s="14"/>
-      <c r="N30" s="14"/>
-      <c r="O30" s="14"/>
-      <c r="P30" s="14"/>
-      <c r="Q30" s="14"/>
-      <c r="R30" s="14"/>
-      <c r="S30" s="15"/>
-    </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="G31" s="19"/>
-      <c r="H31" s="14"/>
-      <c r="I31" s="14"/>
-      <c r="J31" s="14"/>
-      <c r="K31" s="14"/>
-      <c r="L31" s="14"/>
-      <c r="M31" s="14"/>
-      <c r="N31" s="14"/>
-      <c r="O31" s="14"/>
-      <c r="P31" s="14"/>
-      <c r="Q31" s="14"/>
-      <c r="R31" s="14"/>
-      <c r="S31" s="15"/>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="B32" s="3" t="s">
+      <c r="D29" s="46"/>
+      <c r="G29" s="16"/>
+      <c r="H29" s="11"/>
+      <c r="I29" s="11"/>
+      <c r="J29" s="11"/>
+      <c r="K29" s="11"/>
+      <c r="L29" s="11"/>
+      <c r="M29" s="11"/>
+      <c r="N29" s="11"/>
+      <c r="O29" s="11"/>
+      <c r="P29" s="11"/>
+      <c r="Q29" s="11"/>
+      <c r="R29" s="11"/>
+      <c r="S29" s="12"/>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="G30" s="16"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="11"/>
+      <c r="J30" s="11"/>
+      <c r="K30" s="11"/>
+      <c r="L30" s="11"/>
+      <c r="M30" s="11"/>
+      <c r="N30" s="11"/>
+      <c r="O30" s="11"/>
+      <c r="P30" s="11"/>
+      <c r="Q30" s="11"/>
+      <c r="R30" s="11"/>
+      <c r="S30" s="12"/>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="G31" s="16"/>
+      <c r="H31" s="11"/>
+      <c r="I31" s="11"/>
+      <c r="J31" s="11"/>
+      <c r="K31" s="11"/>
+      <c r="L31" s="11"/>
+      <c r="M31" s="11"/>
+      <c r="N31" s="11"/>
+      <c r="O31" s="11"/>
+      <c r="P31" s="11"/>
+      <c r="Q31" s="11"/>
+      <c r="R31" s="11"/>
+      <c r="S31" s="12"/>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="B32" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="C32" s="4"/>
-      <c r="D32" s="5"/>
-      <c r="G32" s="19"/>
-      <c r="H32" s="14"/>
-      <c r="I32" s="14"/>
-      <c r="J32" s="14"/>
-      <c r="K32" s="14"/>
-      <c r="L32" s="14"/>
-      <c r="M32" s="14"/>
-      <c r="N32" s="14"/>
-      <c r="O32" s="14"/>
-      <c r="P32" s="14"/>
-      <c r="Q32" s="14"/>
-      <c r="R32" s="14"/>
-      <c r="S32" s="15"/>
-    </row>
-    <row r="33" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B33" s="21"/>
-      <c r="C33" s="25"/>
-      <c r="D33" s="26"/>
-      <c r="G33" s="19"/>
-      <c r="H33" s="14"/>
-      <c r="I33" s="14"/>
-      <c r="J33" s="14"/>
-      <c r="K33" s="14"/>
-      <c r="L33" s="14"/>
-      <c r="M33" s="14"/>
-      <c r="N33" s="14"/>
-      <c r="O33" s="14"/>
-      <c r="P33" s="14"/>
-      <c r="Q33" s="14"/>
-      <c r="R33" s="14"/>
-      <c r="S33" s="15"/>
-    </row>
-    <row r="34" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B34" s="21"/>
-      <c r="C34" s="25"/>
-      <c r="D34" s="26"/>
-      <c r="G34" s="19"/>
-      <c r="H34" s="14"/>
-      <c r="I34" s="14"/>
-      <c r="J34" s="14"/>
-      <c r="K34" s="14"/>
-      <c r="L34" s="14"/>
-      <c r="M34" s="14"/>
-      <c r="N34" s="14"/>
-      <c r="O34" s="14"/>
-      <c r="P34" s="14"/>
-      <c r="Q34" s="14"/>
-      <c r="R34" s="14"/>
-      <c r="S34" s="15"/>
-    </row>
-    <row r="35" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B35" s="21"/>
-      <c r="C35" s="25"/>
-      <c r="D35" s="26"/>
-      <c r="G35" s="19"/>
-      <c r="H35" s="14"/>
-      <c r="I35" s="14"/>
-      <c r="J35" s="14"/>
-      <c r="K35" s="14"/>
-      <c r="L35" s="14"/>
-      <c r="M35" s="14"/>
-      <c r="N35" s="14"/>
-      <c r="O35" s="14"/>
-      <c r="P35" s="14"/>
-      <c r="Q35" s="14"/>
-      <c r="R35" s="14"/>
-      <c r="S35" s="15"/>
-    </row>
-    <row r="36" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B36" s="21"/>
-      <c r="C36" s="25"/>
-      <c r="D36" s="26"/>
-      <c r="G36" s="19"/>
-      <c r="H36" s="14"/>
-      <c r="I36" s="14"/>
-      <c r="J36" s="14"/>
-      <c r="K36" s="14"/>
-      <c r="L36" s="14"/>
-      <c r="M36" s="14"/>
-      <c r="N36" s="14"/>
-      <c r="O36" s="14"/>
-      <c r="P36" s="14"/>
-      <c r="Q36" s="14"/>
-      <c r="R36" s="14"/>
-      <c r="S36" s="15"/>
-    </row>
-    <row r="37" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B37" s="22"/>
-      <c r="C37" s="27"/>
-      <c r="D37" s="28"/>
-      <c r="G37" s="20"/>
-      <c r="H37" s="17"/>
-      <c r="I37" s="17"/>
-      <c r="J37" s="17"/>
-      <c r="K37" s="17"/>
-      <c r="L37" s="17"/>
-      <c r="M37" s="17"/>
-      <c r="N37" s="17"/>
-      <c r="O37" s="17"/>
-      <c r="P37" s="17"/>
-      <c r="Q37" s="17"/>
-      <c r="R37" s="17"/>
-      <c r="S37" s="18"/>
+      <c r="C32" s="48"/>
+      <c r="D32" s="49"/>
+      <c r="G32" s="16"/>
+      <c r="H32" s="11"/>
+      <c r="I32" s="11"/>
+      <c r="J32" s="11"/>
+      <c r="K32" s="11"/>
+      <c r="L32" s="11"/>
+      <c r="M32" s="11"/>
+      <c r="N32" s="11"/>
+      <c r="O32" s="11"/>
+      <c r="P32" s="11"/>
+      <c r="Q32" s="11"/>
+      <c r="R32" s="11"/>
+      <c r="S32" s="12"/>
+    </row>
+    <row r="33" spans="2:19" x14ac:dyDescent="0.15">
+      <c r="B33" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="C33" s="53">
+        <f>'Financial Model'!K76</f>
+        <v>0.20742534761796225</v>
+      </c>
+      <c r="D33" s="54"/>
+      <c r="G33" s="16"/>
+      <c r="H33" s="11"/>
+      <c r="I33" s="11"/>
+      <c r="J33" s="11"/>
+      <c r="K33" s="11"/>
+      <c r="L33" s="11"/>
+      <c r="M33" s="11"/>
+      <c r="N33" s="11"/>
+      <c r="O33" s="11"/>
+      <c r="P33" s="11"/>
+      <c r="Q33" s="11"/>
+      <c r="R33" s="11"/>
+      <c r="S33" s="12"/>
+    </row>
+    <row r="34" spans="2:19" x14ac:dyDescent="0.15">
+      <c r="B34" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="C34" s="41"/>
+      <c r="D34" s="42"/>
+      <c r="G34" s="16"/>
+      <c r="H34" s="11"/>
+      <c r="I34" s="11"/>
+      <c r="J34" s="11"/>
+      <c r="K34" s="11"/>
+      <c r="L34" s="11"/>
+      <c r="M34" s="11"/>
+      <c r="N34" s="11"/>
+      <c r="O34" s="11"/>
+      <c r="P34" s="11"/>
+      <c r="Q34" s="11"/>
+      <c r="R34" s="11"/>
+      <c r="S34" s="12"/>
+    </row>
+    <row r="35" spans="2:19" x14ac:dyDescent="0.15">
+      <c r="B35" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="C35" s="41"/>
+      <c r="D35" s="42"/>
+      <c r="G35" s="16"/>
+      <c r="H35" s="11"/>
+      <c r="I35" s="11"/>
+      <c r="J35" s="11"/>
+      <c r="K35" s="11"/>
+      <c r="L35" s="11"/>
+      <c r="M35" s="11"/>
+      <c r="N35" s="11"/>
+      <c r="O35" s="11"/>
+      <c r="P35" s="11"/>
+      <c r="Q35" s="11"/>
+      <c r="R35" s="11"/>
+      <c r="S35" s="12"/>
+    </row>
+    <row r="36" spans="2:19" x14ac:dyDescent="0.15">
+      <c r="B36" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="C36" s="41"/>
+      <c r="D36" s="42"/>
+      <c r="G36" s="16"/>
+      <c r="H36" s="11"/>
+      <c r="I36" s="11"/>
+      <c r="J36" s="11"/>
+      <c r="K36" s="11"/>
+      <c r="L36" s="11"/>
+      <c r="M36" s="11"/>
+      <c r="N36" s="11"/>
+      <c r="O36" s="11"/>
+      <c r="P36" s="11"/>
+      <c r="Q36" s="11"/>
+      <c r="R36" s="11"/>
+      <c r="S36" s="12"/>
+    </row>
+    <row r="37" spans="2:19" x14ac:dyDescent="0.15">
+      <c r="B37" s="17"/>
+      <c r="C37" s="43"/>
+      <c r="D37" s="44"/>
+      <c r="G37" s="17"/>
+      <c r="H37" s="14"/>
+      <c r="I37" s="14"/>
+      <c r="J37" s="14"/>
+      <c r="K37" s="14"/>
+      <c r="L37" s="14"/>
+      <c r="M37" s="14"/>
+      <c r="N37" s="14"/>
+      <c r="O37" s="14"/>
+      <c r="P37" s="14"/>
+      <c r="Q37" s="14"/>
+      <c r="R37" s="14"/>
+      <c r="S37" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C37:D37"/>
     <mergeCell ref="C26:D26"/>
     <mergeCell ref="C27:D27"/>
     <mergeCell ref="C29:D29"/>
@@ -1782,240 +1866,246 @@
     <mergeCell ref="C25:D25"/>
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C37:D37"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C29:D29" r:id="rId1" display="Link" xr:uid="{5421A33A-B86C-4727-9FDA-EA3E30BFBF6A}"/>
+    <hyperlink ref="H22" r:id="rId2" xr:uid="{30AC97B8-6A64-A74C-90DA-59D3198B2670}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId2"/>
-  <drawing r:id="rId3"/>
+  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId3"/>
+  <drawing r:id="rId4"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{189A0F92-CF5D-4546-9777-39819DEC72FB}">
-  <dimension ref="B1:U69"/>
+  <dimension ref="B1:U79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C19" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C50" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="F32" sqref="F32"/>
+      <selection pane="bottomRight" activeCell="I62" sqref="I62:I63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="5.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="30.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="9" width="9.140625" style="1"/>
-    <col min="10" max="10" width="9.140625" style="46"/>
-    <col min="11" max="11" width="9.140625" style="1"/>
-    <col min="12" max="12" width="9.140625" style="46"/>
-    <col min="13" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="5.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="30.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="9" width="9.1640625" style="1"/>
+    <col min="10" max="10" width="9.1640625" style="33"/>
+    <col min="11" max="11" width="9.1640625" style="1"/>
+    <col min="12" max="12" width="9.1640625" style="33"/>
+    <col min="13" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:21" s="32" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="I1" s="32" t="s">
+    <row r="1" spans="2:21" s="21" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="I1" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="J1" s="43" t="s">
+      <c r="J1" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="K1" s="37" t="s">
+      <c r="K1" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="L1" s="43" t="s">
+      <c r="L1" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="Q1" s="32" t="s">
+      <c r="Q1" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="R1" s="32" t="s">
+      <c r="R1" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="S1" s="32" t="s">
+      <c r="S1" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="T1" s="32" t="s">
+      <c r="T1" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="U1" s="32" t="s">
+      <c r="U1" s="21" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="33"/>
-      <c r="I2" s="39">
+    <row r="2" spans="2:21" s="23" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B2" s="22"/>
+      <c r="I2" s="26">
         <v>44072</v>
       </c>
-      <c r="J2" s="44"/>
-      <c r="K2" s="39">
+      <c r="J2" s="31"/>
+      <c r="K2" s="26">
         <v>44437</v>
       </c>
-      <c r="L2" s="44"/>
-    </row>
-    <row r="3" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="33"/>
-      <c r="J3" s="44"/>
-      <c r="K3" s="38">
+      <c r="L2" s="31"/>
+    </row>
+    <row r="3" spans="2:21" s="23" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B3" s="22"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="25">
         <v>44600</v>
       </c>
-      <c r="L3" s="44"/>
-    </row>
-    <row r="4" spans="2:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="L3" s="31"/>
+    </row>
+    <row r="4" spans="2:21" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B4" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="I4" s="41">
+      <c r="I4" s="28">
         <v>94.451999999999998</v>
       </c>
-      <c r="J4" s="45"/>
-      <c r="K4" s="41">
+      <c r="J4" s="32"/>
+      <c r="K4" s="28">
         <v>127.871</v>
       </c>
-      <c r="L4" s="45"/>
-    </row>
-    <row r="5" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="L4" s="32"/>
+    </row>
+    <row r="5" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I5" s="42">
+      <c r="I5" s="29">
         <v>47.005000000000003</v>
       </c>
-      <c r="K5" s="42">
+      <c r="K5" s="29">
         <v>63.484000000000002</v>
       </c>
     </row>
-    <row r="6" spans="2:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:21" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B6" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="I6" s="41">
+      <c r="I6" s="28">
         <f>I4-I5</f>
         <v>47.446999999999996</v>
       </c>
-      <c r="J6" s="45"/>
-      <c r="K6" s="41">
+      <c r="J6" s="32"/>
+      <c r="K6" s="28">
         <f>K4-K5</f>
         <v>64.387</v>
       </c>
-      <c r="L6" s="45"/>
-    </row>
-    <row r="7" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B7" s="40" t="s">
+      <c r="L6" s="32"/>
+    </row>
+    <row r="7" spans="2:21" x14ac:dyDescent="0.15">
+      <c r="B7" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="I7" s="42">
+      <c r="I7" s="29">
         <v>44.530999999999999</v>
       </c>
-      <c r="K7" s="42">
+      <c r="K7" s="29">
         <v>60.674999999999997</v>
       </c>
     </row>
-    <row r="8" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B8" s="40" t="s">
+    <row r="8" spans="2:21" x14ac:dyDescent="0.15">
+      <c r="B8" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="I8" s="42">
+      <c r="I8" s="29">
         <v>0.70299999999999996</v>
       </c>
-      <c r="K8" s="42">
+      <c r="K8" s="29">
         <v>0.39600000000000002</v>
       </c>
     </row>
-    <row r="9" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B9" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="I9" s="42">
+      <c r="I9" s="29">
         <f>I7+I8</f>
         <v>45.234000000000002</v>
       </c>
-      <c r="K9" s="42">
+      <c r="K9" s="29">
         <f>K7+K8</f>
         <v>61.070999999999998</v>
       </c>
     </row>
-    <row r="10" spans="2:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:21" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B10" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="I10" s="41">
+      <c r="I10" s="28">
         <f>I6-I9</f>
         <v>2.2129999999999939</v>
       </c>
-      <c r="J10" s="45"/>
-      <c r="K10" s="41">
+      <c r="J10" s="32"/>
+      <c r="K10" s="28">
         <f>K6-K9</f>
         <v>3.3160000000000025</v>
       </c>
-      <c r="L10" s="45"/>
-    </row>
-    <row r="11" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="L10" s="32"/>
+    </row>
+    <row r="11" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B11" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="I11" s="42">
+      <c r="I11" s="29">
         <v>0.88500000000000001</v>
       </c>
-      <c r="K11" s="42">
+      <c r="K11" s="29">
         <v>0.76600000000000001</v>
       </c>
     </row>
-    <row r="12" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B12" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I12" s="42">
+      <c r="I12" s="29">
         <f>I10-I11</f>
         <v>1.3279999999999939</v>
       </c>
-      <c r="K12" s="42">
+      <c r="K12" s="29">
         <f>K10-K11</f>
         <v>2.5500000000000025</v>
       </c>
     </row>
-    <row r="13" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B13" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="I13" s="42">
+      <c r="I13" s="29">
         <v>0.17699999999999999</v>
       </c>
-      <c r="K13" s="42">
+      <c r="K13" s="29">
         <v>0.27800000000000002</v>
       </c>
     </row>
-    <row r="14" spans="2:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:21" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B14" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="I14" s="41">
+      <c r="I14" s="28">
         <f>I12-I13</f>
         <v>1.1509999999999938</v>
       </c>
-      <c r="J14" s="45"/>
-      <c r="K14" s="41">
+      <c r="J14" s="32"/>
+      <c r="K14" s="28">
         <f>K12-K13</f>
         <v>2.2720000000000025</v>
       </c>
-      <c r="L14" s="45"/>
-    </row>
-    <row r="15" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="L14" s="32"/>
+    </row>
+    <row r="15" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B15" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="I15" s="48">
+      <c r="I15" s="35">
         <f>I14/I16</f>
         <v>1.1196498054474648E-2</v>
       </c>
-      <c r="J15" s="49"/>
-      <c r="K15" s="48">
+      <c r="J15" s="36"/>
+      <c r="K15" s="35">
         <f>K14/K16</f>
         <v>2.0598368087035381E-2</v>
       </c>
     </row>
-    <row r="16" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B16" s="1" t="s">
         <v>4</v>
       </c>
@@ -2026,343 +2116,575 @@
         <v>110.3</v>
       </c>
     </row>
-    <row r="18" spans="2:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:21" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B18" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="J18" s="45"/>
-      <c r="K18" s="47">
+      <c r="J18" s="32"/>
+      <c r="K18" s="34">
         <f>K4/I4-1</f>
         <v>0.35381992969974174</v>
       </c>
-      <c r="L18" s="45"/>
-    </row>
-    <row r="19" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="L18" s="32"/>
+    </row>
+    <row r="19" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B19" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="Q19" s="31" t="s">
+      <c r="Q19" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="R19" s="31" t="s">
+      <c r="R19" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="S19" s="31" t="s">
+      <c r="S19" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="T19" s="31" t="s">
+      <c r="T19" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="U19" s="31" t="s">
+      <c r="U19" s="20" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="21" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B21" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="I21" s="50">
+      <c r="I21" s="37">
         <f>I6/I4</f>
         <v>0.50233981281497475</v>
       </c>
-      <c r="K21" s="50">
+      <c r="K21" s="37">
         <f>K6/K4</f>
         <v>0.50353090223741115</v>
       </c>
     </row>
-    <row r="22" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B22" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="I22" s="50">
+      <c r="I22" s="37">
         <f>I10/I4</f>
         <v>2.3429890314657115E-2</v>
       </c>
-      <c r="K22" s="50">
+      <c r="K22" s="37">
         <f>K10/K4</f>
         <v>2.5932384981739429E-2</v>
       </c>
     </row>
-    <row r="23" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B23" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="I23" s="50">
+      <c r="I23" s="37">
         <f>I14/I4</f>
         <v>1.2186083936814401E-2</v>
       </c>
-      <c r="K23" s="50">
+      <c r="K23" s="37">
         <f>K14/K4</f>
         <v>1.7767906718489747E-2</v>
       </c>
     </row>
-    <row r="24" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B24" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="I24" s="50">
+      <c r="I24" s="37">
         <f>I13/I12</f>
         <v>0.13328313253012108</v>
       </c>
-      <c r="K24" s="50">
+      <c r="K24" s="37">
         <f>K13/K12</f>
         <v>0.10901960784313716</v>
       </c>
     </row>
-    <row r="28" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B28" s="51" t="s">
+    <row r="28" spans="2:21" x14ac:dyDescent="0.15">
+      <c r="B28" s="38" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="29" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B29" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="K29" s="42">
+      <c r="I29" s="29">
+        <v>18.748000000000001</v>
+      </c>
+      <c r="K29" s="29">
         <f>5.531+25.598</f>
         <v>31.128999999999998</v>
       </c>
     </row>
-    <row r="30" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B30" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="K30" s="42">
+      <c r="I30" s="29">
+        <v>23.667999999999999</v>
+      </c>
+      <c r="K30" s="29">
         <v>29.561</v>
       </c>
     </row>
-    <row r="31" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B31" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="K31" s="42">
+      <c r="I31" s="29">
+        <v>32.344000000000001</v>
+      </c>
+      <c r="K31" s="29">
         <v>28.315000000000001</v>
       </c>
     </row>
-    <row r="32" spans="2:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:21" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B32" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="J32" s="45"/>
-      <c r="K32" s="41">
+      <c r="I32" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J32" s="32"/>
+      <c r="K32" s="28">
         <v>9.2999999999999999E-2</v>
       </c>
-      <c r="L32" s="45"/>
-    </row>
-    <row r="33" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="L32" s="32"/>
+    </row>
+    <row r="33" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B33" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="K33" s="42">
+      <c r="I33" s="29">
+        <v>2.831</v>
+      </c>
+      <c r="K33" s="29">
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B34" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="K34" s="42">
+      <c r="I34" s="29">
+        <f>SUM(I29:I33)</f>
+        <v>77.61099999999999</v>
+      </c>
+      <c r="K34" s="29">
         <f>SUM(K29:K33)</f>
         <v>89.097999999999999</v>
       </c>
     </row>
-    <row r="35" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B35" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="J35" s="45"/>
-      <c r="K35" s="41">
+      <c r="I35" s="28">
+        <v>42.704000000000001</v>
+      </c>
+      <c r="J35" s="32"/>
+      <c r="K35" s="28">
         <v>61.878</v>
       </c>
-      <c r="L35" s="45"/>
-    </row>
-    <row r="36" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="L35" s="32"/>
+    </row>
+    <row r="36" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B36" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="K36" s="42">
+      <c r="I36" s="29">
+        <v>1.6140000000000001</v>
+      </c>
+      <c r="K36" s="29">
         <v>1.591</v>
       </c>
     </row>
-    <row r="37" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B37" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="K37" s="42">
+      <c r="I37" s="29">
+        <v>13.471</v>
+      </c>
+      <c r="K37" s="29">
         <v>21.268000000000001</v>
       </c>
     </row>
-    <row r="38" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B38" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J38" s="45"/>
-      <c r="K38" s="41">
+      <c r="I38" s="28">
+        <v>28.577000000000002</v>
+      </c>
+      <c r="J38" s="32"/>
+      <c r="K38" s="28">
         <v>17.032</v>
       </c>
-      <c r="L38" s="45"/>
-    </row>
-    <row r="39" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="L38" s="32"/>
+    </row>
+    <row r="39" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B39" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="J39" s="45"/>
-      <c r="K39" s="41">
+      <c r="I39" s="28">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="J39" s="32"/>
+      <c r="K39" s="28">
         <v>2.226</v>
       </c>
-      <c r="L39" s="45"/>
-    </row>
-    <row r="40" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="L39" s="32"/>
+    </row>
+    <row r="40" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B40" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="K40" s="42">
+      <c r="I40" s="29">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="K40" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B41" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="K41" s="42">
+      <c r="I41" s="29">
+        <f>SUM(I35:I40)+I34</f>
+        <v>164.108</v>
+      </c>
+      <c r="K41" s="29">
         <f>SUM(K35:K40)+K34</f>
         <v>193.09299999999999</v>
       </c>
     </row>
-    <row r="43" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="K42" s="29"/>
+    </row>
+    <row r="43" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B43" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="K43" s="1">
+      <c r="I43" s="29">
+        <v>56.731000000000002</v>
+      </c>
+      <c r="K43" s="29">
         <v>69.251000000000005</v>
       </c>
     </row>
-    <row r="44" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B44" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="K44" s="1">
+      <c r="I44" s="29">
+        <v>10.484999999999999</v>
+      </c>
+      <c r="K44" s="29">
         <v>9.7539999999999996</v>
       </c>
     </row>
-    <row r="45" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B45" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="K45" s="1">
+      <c r="I45" s="29">
+        <v>0.998</v>
+      </c>
+      <c r="K45" s="29">
         <v>9.8000000000000004E-2</v>
       </c>
     </row>
-    <row r="46" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B46" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="J46" s="45"/>
-      <c r="L46" s="45"/>
-    </row>
-    <row r="47" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="I46" s="28">
+        <v>4.3959999999999999</v>
+      </c>
+      <c r="J46" s="32"/>
+      <c r="K46" s="28">
+        <v>14.148999999999999</v>
+      </c>
+      <c r="L46" s="32"/>
+    </row>
+    <row r="47" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B47" s="1" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="48" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="I47" s="29">
+        <v>2.4649999999999999</v>
+      </c>
+      <c r="K47" s="29">
+        <v>2.9020000000000001</v>
+      </c>
+    </row>
+    <row r="48" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B48" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="49" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="I48" s="29">
+        <v>3.7679999999999998</v>
+      </c>
+      <c r="K48" s="29">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="49" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B49" s="1" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="50" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I49" s="29">
+        <v>0</v>
+      </c>
+      <c r="K49" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B50" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="J50" s="45"/>
-      <c r="L50" s="45"/>
-    </row>
-    <row r="51" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I50" s="28">
+        <v>0</v>
+      </c>
+      <c r="J50" s="32"/>
+      <c r="K50" s="28">
+        <v>0</v>
+      </c>
+      <c r="L50" s="32"/>
+    </row>
+    <row r="51" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B51" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="J51" s="45"/>
-      <c r="L51" s="45"/>
-    </row>
-    <row r="52" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="I51" s="28">
+        <v>0</v>
+      </c>
+      <c r="J51" s="32"/>
+      <c r="K51" s="28">
+        <v>3.4550000000000001</v>
+      </c>
+      <c r="L51" s="32"/>
+    </row>
+    <row r="52" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B52" s="1" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="53" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I52" s="29">
+        <f>SUM(I43:I51)</f>
+        <v>78.843000000000018</v>
+      </c>
+      <c r="K52" s="29">
+        <f>SUM(K43:K51)</f>
+        <v>103.30900000000001</v>
+      </c>
+    </row>
+    <row r="53" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B53" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="J53" s="45"/>
-      <c r="L53" s="45"/>
-    </row>
-    <row r="54" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="I53" s="28">
+        <v>8.5329999999999995</v>
+      </c>
+      <c r="J53" s="32"/>
+      <c r="K53" s="28">
+        <v>8.2520000000000007</v>
+      </c>
+      <c r="L53" s="32"/>
+    </row>
+    <row r="54" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B54" s="1" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="55" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="I54" s="29">
+        <v>34.46</v>
+      </c>
+      <c r="K54" s="29">
+        <v>28.396999999999998</v>
+      </c>
+    </row>
+    <row r="55" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B55" s="1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="56" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="I55" s="29">
+        <v>0</v>
+      </c>
+      <c r="K55" s="29">
+        <v>0.49099999999999999</v>
+      </c>
+    </row>
+    <row r="56" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B56" s="1" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="57" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="I56" s="29">
+        <v>1.228</v>
+      </c>
+      <c r="K56" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B57" s="1" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="59" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="I57" s="29">
+        <f>I52+SUM(I53:I56)</f>
+        <v>123.06400000000002</v>
+      </c>
+      <c r="K57" s="29">
+        <f>K52+SUM(K53:K56)</f>
+        <v>140.44900000000001</v>
+      </c>
+    </row>
+    <row r="59" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B59" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="60" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="I59" s="29">
+        <v>41.043999999999997</v>
+      </c>
+      <c r="K59" s="29">
+        <v>52.643999999999998</v>
+      </c>
+    </row>
+    <row r="60" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B60" s="1" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="62" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="I60" s="29">
+        <f>I59+I57</f>
+        <v>164.108</v>
+      </c>
+      <c r="K60" s="29">
+        <f>K59+K57</f>
+        <v>193.09300000000002</v>
+      </c>
+    </row>
+    <row r="62" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B62" s="1" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="63" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="I62" s="29">
+        <f>I41-I57</f>
+        <v>41.043999999999983</v>
+      </c>
+      <c r="K62" s="29">
+        <f>K41-K57</f>
+        <v>52.643999999999977</v>
+      </c>
+    </row>
+    <row r="63" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B63" s="1" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="65" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B65" s="1" t="s">
+      <c r="I63" s="1">
+        <f>I62/I16</f>
+        <v>0.39926070038910488</v>
+      </c>
+      <c r="K63" s="1">
+        <f>K62/K16</f>
+        <v>0.47728014505893002</v>
+      </c>
+    </row>
+    <row r="65" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B65" s="2" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="67" spans="2:12" s="52" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B67" s="52" t="s">
+      <c r="J65" s="32"/>
+      <c r="K65" s="34">
+        <f>K35/I35-1</f>
+        <v>0.44899775196702874</v>
+      </c>
+      <c r="L65" s="32"/>
+    </row>
+    <row r="66" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B66" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="68" spans="2:12" s="39" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B68" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="J67" s="53"/>
-      <c r="L67" s="53"/>
-    </row>
-    <row r="68" spans="2:12" s="52" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B68" s="52" t="s">
+      <c r="J68" s="40"/>
+      <c r="K68" s="50">
+        <f>K39+K38+K32</f>
+        <v>19.350999999999999</v>
+      </c>
+      <c r="L68" s="40"/>
+    </row>
+    <row r="69" spans="2:12" s="39" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B69" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="J68" s="53"/>
-      <c r="L68" s="53"/>
-    </row>
-    <row r="69" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B69" s="1" t="s">
+      <c r="J69" s="40"/>
+      <c r="K69" s="50">
+        <f>K46+K50+K51+K53</f>
+        <v>25.856000000000002</v>
+      </c>
+      <c r="L69" s="40"/>
+    </row>
+    <row r="70" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B70" s="1" t="s">
         <v>8</v>
+      </c>
+      <c r="K70" s="29">
+        <f>K68-K69</f>
+        <v>-6.5050000000000026</v>
+      </c>
+    </row>
+    <row r="72" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B72" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="K72" s="52">
+        <v>9.9000000000000005E-2</v>
+      </c>
+    </row>
+    <row r="73" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B73" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K73" s="29">
+        <f>K72*K16</f>
+        <v>10.919700000000001</v>
+      </c>
+    </row>
+    <row r="74" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B74" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K74" s="29">
+        <f>K73-K70</f>
+        <v>17.424700000000001</v>
+      </c>
+    </row>
+    <row r="76" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B76" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="K76" s="51">
+        <f>K72/K63</f>
+        <v>0.20742534761796225</v>
+      </c>
+    </row>
+    <row r="77" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B77" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="78" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B78" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="79" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B79" s="1" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>